<commit_message>
v2.0 - Implemented Builder design pattern for do_graph function
</commit_message>
<xml_diff>
--- a/data_src/excel_file_2.xlsx
+++ b/data_src/excel_file_2.xlsx
@@ -7689,6 +7689,27 @@
       </c>
     </row>
     <row r="56" spans="1:3150">
+      <c r="A56" t="s">
+        <v>0</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1</v>
+      </c>
+      <c r="C56" t="n">
+        <v>42</v>
+      </c>
+      <c r="D56" t="n">
+        <v>666</v>
+      </c>
+      <c r="E56" t="s">
+        <v>2</v>
+      </c>
+      <c r="F56" t="n">
+        <v>180</v>
+      </c>
+      <c r="G56" t="s">
+        <v>16</v>
+      </c>
       <c r="MM56" t="s">
         <v>103</v>
       </c>
@@ -7793,6 +7814,27 @@
       </c>
     </row>
     <row r="57" spans="1:3150">
+      <c r="A57" t="s">
+        <v>0</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57" t="n">
+        <v>42</v>
+      </c>
+      <c r="D57" t="n">
+        <v>666</v>
+      </c>
+      <c r="E57" t="s">
+        <v>2</v>
+      </c>
+      <c r="F57" t="n">
+        <v>180</v>
+      </c>
+      <c r="G57" t="s">
+        <v>16</v>
+      </c>
       <c r="MT57" t="s">
         <v>105</v>
       </c>
@@ -7897,6 +7939,27 @@
       </c>
     </row>
     <row r="58" spans="1:3150">
+      <c r="A58" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" t="n">
+        <v>42</v>
+      </c>
+      <c r="D58" t="n">
+        <v>666</v>
+      </c>
+      <c r="E58" t="s">
+        <v>2</v>
+      </c>
+      <c r="F58" t="n">
+        <v>180</v>
+      </c>
+      <c r="G58" t="s">
+        <v>16</v>
+      </c>
       <c r="NA58" t="s">
         <v>106</v>
       </c>
@@ -8004,6 +8067,27 @@
       </c>
     </row>
     <row r="59" spans="1:3150">
+      <c r="A59" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59" t="n">
+        <v>42</v>
+      </c>
+      <c r="D59" t="n">
+        <v>666</v>
+      </c>
+      <c r="E59" t="s">
+        <v>2</v>
+      </c>
+      <c r="F59" t="n">
+        <v>180</v>
+      </c>
+      <c r="G59" t="s">
+        <v>16</v>
+      </c>
       <c r="NH59" t="s">
         <v>108</v>
       </c>
@@ -8111,6 +8195,27 @@
       </c>
     </row>
     <row r="60" spans="1:3150">
+      <c r="A60" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1</v>
+      </c>
+      <c r="C60" t="n">
+        <v>42</v>
+      </c>
+      <c r="D60" t="n">
+        <v>666</v>
+      </c>
+      <c r="E60" t="s">
+        <v>2</v>
+      </c>
+      <c r="F60" t="n">
+        <v>180</v>
+      </c>
+      <c r="G60" t="s">
+        <v>16</v>
+      </c>
       <c r="NO60" t="s">
         <v>110</v>
       </c>
@@ -8218,6 +8323,27 @@
       </c>
     </row>
     <row r="61" spans="1:3150">
+      <c r="A61" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" t="n">
+        <v>42</v>
+      </c>
+      <c r="D61" t="n">
+        <v>666</v>
+      </c>
+      <c r="E61" t="s">
+        <v>2</v>
+      </c>
+      <c r="F61" t="n">
+        <v>180</v>
+      </c>
+      <c r="G61" t="s">
+        <v>16</v>
+      </c>
       <c r="NV61" t="s">
         <v>112</v>
       </c>
@@ -8322,6 +8448,27 @@
       </c>
     </row>
     <row r="62" spans="1:3150">
+      <c r="A62" t="s">
+        <v>0</v>
+      </c>
+      <c r="B62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C62" t="n">
+        <v>42</v>
+      </c>
+      <c r="D62" t="n">
+        <v>666</v>
+      </c>
+      <c r="E62" t="s">
+        <v>2</v>
+      </c>
+      <c r="F62" t="n">
+        <v>180</v>
+      </c>
+      <c r="G62" t="s">
+        <v>16</v>
+      </c>
       <c r="OC62" t="s">
         <v>114</v>
       </c>
@@ -8426,6 +8573,27 @@
       </c>
     </row>
     <row r="63" spans="1:3150">
+      <c r="A63" t="s">
+        <v>0</v>
+      </c>
+      <c r="B63" t="s">
+        <v>1</v>
+      </c>
+      <c r="C63" t="n">
+        <v>42</v>
+      </c>
+      <c r="D63" t="n">
+        <v>666</v>
+      </c>
+      <c r="E63" t="s">
+        <v>2</v>
+      </c>
+      <c r="F63" t="n">
+        <v>180</v>
+      </c>
+      <c r="G63" t="s">
+        <v>16</v>
+      </c>
       <c r="OJ63" t="s">
         <v>116</v>
       </c>

</xml_diff>